<commit_message>
修改微车一级用例 by Travis @20131016
</commit_message>
<xml_diff>
--- a/Buding_Primary_TestCases/布丁微车v2.4.1测试用例(一级).xlsx
+++ b/Buding_Primary_TestCases/布丁微车v2.4.1测试用例(一级).xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="启动A" sheetId="4" r:id="rId1"/>
+    <sheet name="车辆管理B" sheetId="5" r:id="rId2"/>
+    <sheet name="账户与设置" sheetId="2" r:id="rId3"/>
+    <sheet name="消息分享" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>测试项</t>
   </si>
@@ -128,12 +130,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>007</t>
-  </si>
-  <si>
-    <t>008</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. 进入消息盒子页面
 2. 点击任意消息，进入消息详情页
 3. 点击右上角分享按钮，选择“微博”，跳转至微博
@@ -153,6 +149,85 @@
 2. 消息存在pic时显示该pic预览，图片分辨率、尺寸显示适中；不存在pic时，不显示
 3. 消息内容显示完整，无错字，显示不全等问题
 4. 消息中不显示url链接内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>应用启动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 应用可成功启动
+2. 首页数据【新增、高发、车辆信息、消息】加载正常
+3. 账户状态正常</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 点击手机桌面微车icon
+2. 查看</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>启动A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>车辆管理B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加车辆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除车辆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>编辑车辆</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>测试设备已联网(不关心网络环境)</t>
+  </si>
+  <si>
+    <t>1. 页面显示butterfly loading动画
+2. loading结束后，车辆添加成功，跳转至“车辆违章列表”页面，页面list处于加载状态
+3. 加载完成后
+  a. 如果车辆存在违章则显示违章；
+  b. 如果车辆不存在违章，且车辆信息正确，则显示“恭喜您，暂时没有违章”提示；
+  c. 如果车辆信息错误，则显示“车辆信息错误”提示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 进入应用首页，点击任意已添加车辆区域的车型图片
+2. 修改车辆信息【车型图片、车辆信息】
+3. 点击“保存”按钮
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 进入应用首页，点击“添加车辆”入口
+2. 选择查询城市并输入必填车辆信息
+3. 点击“保存”按钮
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 页面返回应用首页
+2. 查看该车辆已被删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 进入应用首页，点击任意已添加车辆区域的车型图片
+2. 点击页面右上角“删除”按钮
+3. 点击“确定”按钮
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -213,7 +288,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -221,19 +296,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -243,9 +330,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -256,13 +340,127 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -577,185 +775,484 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="11.875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="7" customWidth="1"/>
-    <col min="3" max="4" width="16.375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="31.125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="61.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="11.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.875" style="5" customWidth="1"/>
+    <col min="3" max="4" width="16.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="61.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:7" ht="49.5">
+      <c r="A2" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="2"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G3:G4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+      <formula1>"N,F,P"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+      <formula1>"测试设备已联网(不关心网络环境),测试设备未联网,测试设备连接可用Wifi,测试设备连接2G,测试设备连接3G,测试设备连接无外网Wifi"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="11.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.875" style="5" customWidth="1"/>
+    <col min="3" max="4" width="16.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="61.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="132">
+      <c r="A2" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" ht="132">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" spans="1:7" ht="99">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="A2:A4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"P"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+      <formula1>"N,F,P"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
+      <formula1>"测试设备已联网(不关心网络环境),测试设备未联网,测试设备连接可用Wifi,测试设备连接2G,测试设备连接3G,测试设备连接无外网Wifi"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="1" width="11.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.875" style="5" customWidth="1"/>
+    <col min="3" max="4" width="16.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="61.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2" spans="1:7" ht="99">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" ht="115.5">
-      <c r="A3" s="9"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="4" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="1:7" ht="99">
-      <c r="A4" s="9"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="12"/>
+    </row>
+    <row r="5" spans="1:7" ht="115.5">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C5" s="10"/>
+      <c r="D5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="10"/>
+      <c r="F5" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" ht="66">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="115.5">
-      <c r="A5" s="9"/>
-      <c r="B5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="4" t="s">
+      <c r="E6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" spans="1:7" ht="66">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="66">
-      <c r="A6" s="9"/>
-      <c r="B6" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="66">
-      <c r="A7" s="9"/>
-      <c r="B7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="9"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="4"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="9"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="4"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="3"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -770,10 +1267,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G1:G1048576">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"P"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -787,21 +1284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>